<commit_message>
feat:update calculation of relatedness between section and city
</commit_message>
<xml_diff>
--- a/data_sample.xlsx
+++ b/data_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\PycharmProjects\economic_compound_index\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4FA543-1215-4C53-8C80-E7B6664E0E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592D43D2-9243-446E-A233-92DEE3D34EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -352,7 +352,7 @@
   <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -379,8 +379,8 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <f ca="1">RANDBETWEEN(0, 1000)</f>
-        <v>461</v>
+        <f ca="1">RANDBETWEEN(0, 500)</f>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -391,8 +391,8 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C57" ca="1" si="0">RANDBETWEEN(0, 1000)</f>
-        <v>690</v>
+        <f t="shared" ref="C3:C17" ca="1" si="0">RANDBETWEEN(0, 500)</f>
+        <v>419</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -404,7 +404,7 @@
       </c>
       <c r="C4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>697</v>
+        <v>366</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -416,7 +416,7 @@
       </c>
       <c r="C5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>160</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -428,7 +428,7 @@
       </c>
       <c r="C6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>336</v>
+        <v>461</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -440,7 +440,7 @@
       </c>
       <c r="C7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -452,7 +452,7 @@
       </c>
       <c r="C8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>284</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -464,7 +464,7 @@
       </c>
       <c r="C9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>454</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -476,7 +476,7 @@
       </c>
       <c r="C10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>431</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -488,7 +488,7 @@
       </c>
       <c r="C11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>751</v>
+        <v>375</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -500,7 +500,7 @@
       </c>
       <c r="C12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>439</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -512,7 +512,7 @@
       </c>
       <c r="C13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>624</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -524,7 +524,7 @@
       </c>
       <c r="C14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>309</v>
+        <v>438</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -536,7 +536,7 @@
       </c>
       <c r="C15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>834</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -548,7 +548,7 @@
       </c>
       <c r="C16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>663</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -560,7 +560,7 @@
       </c>
       <c r="C17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>702</v>
+        <v>344</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -571,8 +571,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>836</v>
+        <v>227</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -583,8 +582,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>222</v>
+        <v>384</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -595,8 +593,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>219</v>
+        <v>235</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -607,8 +604,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>555</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -619,8 +615,7 @@
         <v>5</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>570</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -631,8 +626,7 @@
         <v>6</v>
       </c>
       <c r="C23" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>809</v>
+        <v>235</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -643,8 +637,7 @@
         <v>7</v>
       </c>
       <c r="C24" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>248</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -655,8 +648,7 @@
         <v>8</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>638</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -667,8 +659,8 @@
         <v>1</v>
       </c>
       <c r="C26" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>809</v>
+        <f ca="1">RANDBETWEEN(0, 500)</f>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -679,8 +671,8 @@
         <v>2</v>
       </c>
       <c r="C27" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>620</v>
+        <f t="shared" ref="C27:C57" ca="1" si="1">RANDBETWEEN(0, 500)</f>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -691,8 +683,8 @@
         <v>3</v>
       </c>
       <c r="C28" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>342</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>317</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -703,8 +695,8 @@
         <v>4</v>
       </c>
       <c r="C29" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>911</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>228</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -715,8 +707,8 @@
         <v>5</v>
       </c>
       <c r="C30" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>832</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -727,8 +719,8 @@
         <v>6</v>
       </c>
       <c r="C31" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>573</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>184</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -739,8 +731,8 @@
         <v>7</v>
       </c>
       <c r="C32" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>313</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>471</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -751,8 +743,8 @@
         <v>8</v>
       </c>
       <c r="C33" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>583</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>218</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -763,8 +755,8 @@
         <v>1</v>
       </c>
       <c r="C34" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>663</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>419</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -775,8 +767,8 @@
         <v>2</v>
       </c>
       <c r="C35" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>398</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -787,8 +779,8 @@
         <v>3</v>
       </c>
       <c r="C36" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>281</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -799,8 +791,8 @@
         <v>4</v>
       </c>
       <c r="C37" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>480</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -811,8 +803,8 @@
         <v>5</v>
       </c>
       <c r="C38" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>811</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>373</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -823,8 +815,8 @@
         <v>6</v>
       </c>
       <c r="C39" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>560</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>269</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -835,8 +827,8 @@
         <v>7</v>
       </c>
       <c r="C40" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>443</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>353</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -847,8 +839,8 @@
         <v>8</v>
       </c>
       <c r="C41" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>419</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>471</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -859,8 +851,8 @@
         <v>1</v>
       </c>
       <c r="C42" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>508</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>421</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -871,8 +863,8 @@
         <v>2</v>
       </c>
       <c r="C43" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>761</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -883,8 +875,8 @@
         <v>3</v>
       </c>
       <c r="C44" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>491</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>242</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -895,8 +887,8 @@
         <v>4</v>
       </c>
       <c r="C45" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>168</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -907,8 +899,8 @@
         <v>5</v>
       </c>
       <c r="C46" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>645</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>166</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -919,8 +911,8 @@
         <v>6</v>
       </c>
       <c r="C47" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>792</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>286</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -931,8 +923,8 @@
         <v>7</v>
       </c>
       <c r="C48" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>499</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -943,8 +935,8 @@
         <v>8</v>
       </c>
       <c r="C49" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>432</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -955,8 +947,8 @@
         <v>1</v>
       </c>
       <c r="C50" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>922</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>432</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -967,8 +959,8 @@
         <v>2</v>
       </c>
       <c r="C51" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>277</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>490</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -979,8 +971,8 @@
         <v>3</v>
       </c>
       <c r="C52" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>750</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>467</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -991,8 +983,8 @@
         <v>4</v>
       </c>
       <c r="C53" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>773</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>211</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -1003,8 +995,8 @@
         <v>5</v>
       </c>
       <c r="C54" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>690</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>181</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -1015,8 +1007,8 @@
         <v>6</v>
       </c>
       <c r="C55" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>601</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -1027,8 +1019,8 @@
         <v>7</v>
       </c>
       <c r="C56" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>979</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -1039,8 +1031,8 @@
         <v>8</v>
       </c>
       <c r="C57" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>697</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>